<commit_message>
Fix Class 4 link
</commit_message>
<xml_diff>
--- a/Classes/Class_4/Survey_Exp_Questionnaire_v4.xlsx
+++ b/Classes/Class_4/Survey_Exp_Questionnaire_v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonny\Google Drive\Academic\USP\Teaching\FLS6441 - Methods III\Website\Methods_III\Classes\Class_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCBEB8E-BC08-4181-8F10-04D4F39BF175}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B9C991-116F-4269-B60F-E2DB50AD9757}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="339" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="339" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
   <si>
     <t>type</t>
   </si>
@@ -414,6 +414,21 @@
   </si>
   <si>
     <t>field-list</t>
+  </si>
+  <si>
+    <t>1 pct</t>
+  </si>
+  <si>
+    <t>50 pct</t>
+  </si>
+  <si>
+    <t>5 pct</t>
+  </si>
+  <si>
+    <t>10 pct</t>
+  </si>
+  <si>
+    <t>25 pct</t>
   </si>
 </sst>
 </file>
@@ -863,8 +878,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A350" sqref="A350:D351"/>
       <selection pane="topRight" activeCell="A350" sqref="A350:D351"/>
       <selection pane="bottomLeft" activeCell="A350" sqref="A350:D351"/>
@@ -1114,7 +1129,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1158,7 +1173,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="125" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -1246,10 +1261,10 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A350" sqref="A350:D351"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7265625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1574,8 +1589,8 @@
       <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="2">
-        <v>0.01</v>
+      <c r="C29" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1585,8 +1600,8 @@
       <c r="B30" s="3">
         <v>5</v>
       </c>
-      <c r="C30" s="2">
-        <v>0.05</v>
+      <c r="C30" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1596,8 +1611,8 @@
       <c r="B31" s="3">
         <v>10</v>
       </c>
-      <c r="C31" s="2">
-        <v>0.1</v>
+      <c r="C31" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1607,8 +1622,8 @@
       <c r="B32" s="3">
         <v>20</v>
       </c>
-      <c r="C32" s="2">
-        <v>0.25</v>
+      <c r="C32" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1618,8 +1633,8 @@
       <c r="B33" s="3">
         <v>50</v>
       </c>
-      <c r="C33" s="2">
-        <v>0.5</v>
+      <c r="C33" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update exercise lab 4
</commit_message>
<xml_diff>
--- a/Classes/Class_4/Survey_Exp_Questionnaire_v4.xlsx
+++ b/Classes/Class_4/Survey_Exp_Questionnaire_v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonny\Google Drive\Academic\USP\Teaching\FLS6441 - Methods III\2020\Methods_III\Classes\Class_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C7C59B-65A0-4F1E-A698-7F1E7F2973DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D9C6A9-29E2-4149-8A64-E68EBD0C3135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="339" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
     <t>Conjoint_1.jpg</t>
   </si>
   <si>
-    <t>Cconjoint_4.jpg</t>
+    <t>Conjoint_4.jpg</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1129,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="102" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="89.25" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="127.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="114.75" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>74</v>
       </c>

</xml_diff>